<commit_message>
Adding text, images and restructuring folder
</commit_message>
<xml_diff>
--- a/data/Goederenvervoer_mld_ton_eigen.xlsx
+++ b/data/Goederenvervoer_mld_ton_eigen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jelme\TIL6022\TIL Programming\data\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jelme\TIL6022\Pythongroup8\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{63DFED17-E3C0-4824-8FE5-83882CC9C052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC9B256A-B89D-4929-BEAA-CB23BF503411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3384" yWindow="3360" windowWidth="17280" windowHeight="8880"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Goederenvervoer_mld_ton_eigen" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Trend</t>
   </si>
@@ -42,12 +42,18 @@
   <si>
     <t>Luchtvaart</t>
   </si>
+  <si>
+    <t>https://ec.europa.eu/eurostat/databrowser/view/ttr00009__custom_8071932/default/table?lang=en</t>
+  </si>
+  <si>
+    <t>Statistics | Eurostat (europa.eu)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,6 +184,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -480,7 +494,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -523,11 +537,15 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -556,6 +574,7 @@
     <cellStyle name="Controlecel" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Gekoppelde cel" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Goed" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Invoer" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Kop 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Kop 2" xfId="3" builtinId="17" customBuiltin="1"/>
@@ -880,10 +899,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -1150,7 +1171,19 @@
         <v>44469</v>
       </c>
     </row>
+    <row r="15" spans="1:7" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="C15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C15" r:id="rId1" xr:uid="{A5854E09-0C3A-460E-ADE7-606AA4E47CE9}"/>
+    <hyperlink ref="D15" r:id="rId2" display="https://ec.europa.eu/eurostat/databrowser/view/ttr00009__custom_8071932/default/table?lang=en" xr:uid="{BBAC2E82-02B6-469E-AB52-A535B8EB1413}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>